<commit_message>
finish the normal format to generate code by using the excel file
</commit_message>
<xml_diff>
--- a/Client/Assets/ExcelFiles/Normal.xlsx
+++ b/Client/Assets/ExcelFiles/Normal.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\SimpleUtils\Client\Assets\ExcelFiles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="2715" windowWidth="22770" windowHeight="6915"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="BattleWithScenes" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -916,10 +918,10 @@
   <dimension ref="A1:K50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B31" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2549,34 +2551,4 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
 </file>
</xml_diff>